<commit_message>
r0.3 update 3-sigma line equation
</commit_message>
<xml_diff>
--- a/utils/template.xlsx
+++ b/utils/template.xlsx
@@ -8,17 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaohuag\Documents\py\Data_Handle\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7741531D-CB99-4CA2-A61B-30E4469349AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797AD816-4E4E-47AE-A3BF-C4A99C9A4496}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{DF03CA4E-EB3B-4B9A-AE66-F96449DA53E3}"/>
+    <workbookView xWindow="4404" yWindow="1104" windowWidth="17280" windowHeight="8964" xr2:uid="{DF03CA4E-EB3B-4B9A-AE66-F96449DA53E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Spec" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1453,22 +1450,17 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1486,10 +1478,15 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Accent1" xfId="5" builtinId="30"/>
@@ -2552,23 +2549,9 @@
               <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Versal VC1902 ES2</a:t>
+              <a:t>Spec Line</a:t>
             </a:r>
-            <a:br>
-              <a:rPr lang="en-US"/>
-            </a:br>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>PCIeA#0 Reset, Gen4x8 RP @ </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t>110C</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t> </a:t>
-            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -3045,23 +3028,9 @@
               <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Versal VC1902 ES2</a:t>
+              <a:t>3-sigma Chart</a:t>
             </a:r>
-            <a:br>
-              <a:rPr lang="en-US"/>
-            </a:br>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>PCIeA#0 Reset, Gen4x8 RP @ </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t>110C</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t> </a:t>
-            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -5438,245 +5407,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="ShaoHua"/>
-      <sheetName val="Utility"/>
-      <sheetName val="TILO"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="5">
-          <cell r="J5">
-            <v>7.1006999999999998</v>
-          </cell>
-          <cell r="L5">
-            <v>0.53</v>
-          </cell>
-          <cell r="X5">
-            <v>0.56000000000000005</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="J6">
-            <v>7.1802000000000001</v>
-          </cell>
-          <cell r="L6">
-            <v>0.52</v>
-          </cell>
-          <cell r="X6">
-            <v>0.63</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="J7">
-            <v>7.2797000000000001</v>
-          </cell>
-          <cell r="L7">
-            <v>0.54</v>
-          </cell>
-          <cell r="X7">
-            <v>0.57999999999999996</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="J8">
-            <v>7.2548000000000004</v>
-          </cell>
-          <cell r="L8">
-            <v>0.52</v>
-          </cell>
-          <cell r="X8">
-            <v>0.56000000000000005</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="J9">
-            <v>7.3654999999999999</v>
-          </cell>
-          <cell r="L9">
-            <v>0.53</v>
-          </cell>
-          <cell r="X9">
-            <v>0.56999999999999995</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="J10">
-            <v>7.0366999999999997</v>
-          </cell>
-          <cell r="L10">
-            <v>0.51</v>
-          </cell>
-          <cell r="X10">
-            <v>0.56000000000000005</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="J11">
-            <v>7.6140999999999996</v>
-          </cell>
-          <cell r="L11">
-            <v>0.53</v>
-          </cell>
-          <cell r="X11">
-            <v>0.57999999999999996</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="J12">
-            <v>8.8394999999999992</v>
-          </cell>
-          <cell r="L12">
-            <v>0.57999999999999996</v>
-          </cell>
-          <cell r="X12">
-            <v>0.64</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="J13">
-            <v>9.1380999999999997</v>
-          </cell>
-          <cell r="L13">
-            <v>0.57999999999999996</v>
-          </cell>
-          <cell r="X13">
-            <v>0.64</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="J14">
-            <v>7.7572000000000001</v>
-          </cell>
-          <cell r="L14">
-            <v>0.54</v>
-          </cell>
-          <cell r="X14">
-            <v>0.57999999999999996</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="J15">
-            <v>9.4933999999999994</v>
-          </cell>
-          <cell r="L15">
-            <v>0.57999999999999996</v>
-          </cell>
-          <cell r="X15">
-            <v>0.66</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="J16">
-            <v>9.2236999999999991</v>
-          </cell>
-          <cell r="L16">
-            <v>0.57999999999999996</v>
-          </cell>
-          <cell r="X16">
-            <v>0.65</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="J17">
-            <v>9.0421999999999993</v>
-          </cell>
-          <cell r="L17">
-            <v>0.57999999999999996</v>
-          </cell>
-          <cell r="X17">
-            <v>0.77500000000000002</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="J18">
-            <v>6.0235000000000003</v>
-          </cell>
-          <cell r="L18">
-            <v>0.61</v>
-          </cell>
-          <cell r="X18">
-            <v>0.55000000000000004</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="J19">
-            <v>6.1513</v>
-          </cell>
-          <cell r="L19">
-            <v>0.54</v>
-          </cell>
-          <cell r="X19">
-            <v>0.52</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="J20">
-            <v>6.3197999999999999</v>
-          </cell>
-          <cell r="L20">
-            <v>0.52</v>
-          </cell>
-          <cell r="X20">
-            <v>0.54</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="J21">
-            <v>9.1769999999999996</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="J22">
-            <v>9.3262999999999998</v>
-          </cell>
-          <cell r="X22">
-            <v>0.65</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="J23">
-            <v>9.0632000000000001</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="J24">
-            <v>6.2422000000000004</v>
-          </cell>
-          <cell r="L24">
-            <v>0.66</v>
-          </cell>
-          <cell r="X24">
-            <v>0.53</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="J25">
-            <v>6.1017000000000001</v>
-          </cell>
-          <cell r="L25">
-            <v>0.53</v>
-          </cell>
-          <cell r="X25">
-            <v>0.53</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="J26">
-            <v>6.0511999999999997</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5976,8 +5706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F1EB7E8-9F04-4119-AD4D-6769893E11C2}">
   <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6124,7 +5854,7 @@
         <v>0.61</v>
       </c>
       <c r="Y4" s="24">
-        <f t="shared" ref="Y3:Y23" si="0">X4+3*$X$38</f>
+        <f t="shared" ref="Y4:Y22" si="0">X4+3*$X$38</f>
         <v>0.73</v>
       </c>
     </row>
@@ -6290,7 +6020,7 @@
       <c r="H11" s="24">
         <v>0.67600000000000005</v>
       </c>
-      <c r="I11" s="44"/>
+      <c r="I11" s="32"/>
       <c r="W11" s="24">
         <v>7.7572000000000001</v>
       </c>
@@ -6310,7 +6040,7 @@
       <c r="H12" s="24">
         <v>0.67600000000000005</v>
       </c>
-      <c r="I12" s="44"/>
+      <c r="I12" s="32"/>
       <c r="W12" s="24">
         <v>9.4933999999999994</v>
       </c>
@@ -6330,7 +6060,7 @@
       <c r="H13" s="24">
         <v>0.77500000000000002</v>
       </c>
-      <c r="I13" s="44"/>
+      <c r="I13" s="32"/>
       <c r="W13" s="24">
         <v>9.2236999999999991</v>
       </c>
@@ -6360,7 +6090,7 @@
       <c r="H14" s="24">
         <v>0.77500000000000002</v>
       </c>
-      <c r="I14" s="44"/>
+      <c r="I14" s="32"/>
       <c r="W14" s="24">
         <v>9.0421999999999993</v>
       </c>
@@ -6387,7 +6117,7 @@
       <c r="H15" s="24">
         <v>0.85399999999999998</v>
       </c>
-      <c r="I15" s="44"/>
+      <c r="I15" s="32"/>
       <c r="W15" s="24">
         <v>6.0235000000000003</v>
       </c>
@@ -6417,7 +6147,7 @@
       <c r="H16" s="24">
         <v>0.85399999999999998</v>
       </c>
-      <c r="I16" s="44"/>
+      <c r="I16" s="32"/>
       <c r="W16" s="24">
         <v>6.1513</v>
       </c>
@@ -6600,8 +6330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22CF986A-6963-44BD-AC24-CF6EFFB1083A}">
   <dimension ref="A1:AX42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6634,156 +6364,156 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="43" t="s">
+      <c r="K2" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43" t="s">
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="43" t="s">
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="T2" s="43"/>
-      <c r="U2" s="43"/>
-      <c r="V2" s="43"/>
-      <c r="W2" s="43" t="s">
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="33"/>
+      <c r="W2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="X2" s="43"/>
-      <c r="Y2" s="43"/>
-      <c r="Z2" s="43"/>
-      <c r="AA2" s="35" t="s">
+      <c r="X2" s="33"/>
+      <c r="Y2" s="33"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="AB2" s="36"/>
-      <c r="AC2" s="36"/>
-      <c r="AD2" s="37"/>
-      <c r="AE2" s="35" t="s">
+      <c r="AB2" s="44"/>
+      <c r="AC2" s="44"/>
+      <c r="AD2" s="35"/>
+      <c r="AE2" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="AF2" s="37"/>
-      <c r="AG2" s="35" t="s">
+      <c r="AF2" s="35"/>
+      <c r="AG2" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="AH2" s="37"/>
-      <c r="AI2" s="43" t="s">
+      <c r="AH2" s="35"/>
+      <c r="AI2" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="AJ2" s="43"/>
-      <c r="AK2" s="43"/>
-      <c r="AL2" s="43"/>
-      <c r="AM2" s="43" t="s">
+      <c r="AJ2" s="33"/>
+      <c r="AK2" s="33"/>
+      <c r="AL2" s="33"/>
+      <c r="AM2" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="AN2" s="43"/>
-      <c r="AO2" s="43"/>
-      <c r="AP2" s="43"/>
-      <c r="AQ2" s="43" t="s">
+      <c r="AN2" s="33"/>
+      <c r="AO2" s="33"/>
+      <c r="AP2" s="33"/>
+      <c r="AQ2" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="AR2" s="43"/>
-      <c r="AS2" s="43"/>
-      <c r="AT2" s="43"/>
-      <c r="AU2" s="35"/>
-      <c r="AV2" s="37"/>
-      <c r="AW2" s="35"/>
-      <c r="AX2" s="37"/>
+      <c r="AR2" s="33"/>
+      <c r="AS2" s="33"/>
+      <c r="AT2" s="33"/>
+      <c r="AU2" s="34"/>
+      <c r="AV2" s="35"/>
+      <c r="AW2" s="34"/>
+      <c r="AX2" s="35"/>
     </row>
     <row r="3" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="38"/>
-      <c r="G3" s="39" t="s">
+      <c r="F3" s="37"/>
+      <c r="G3" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="40"/>
-      <c r="I3" s="41" t="s">
+      <c r="H3" s="39"/>
+      <c r="I3" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="42"/>
-      <c r="K3" s="32" t="s">
+      <c r="J3" s="41"/>
+      <c r="K3" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="32"/>
-      <c r="M3" s="33" t="s">
+      <c r="L3" s="36"/>
+      <c r="M3" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="34"/>
-      <c r="O3" s="32" t="s">
+      <c r="N3" s="43"/>
+      <c r="O3" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="33" t="s">
+      <c r="P3" s="36"/>
+      <c r="Q3" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="R3" s="34"/>
-      <c r="S3" s="32" t="s">
+      <c r="R3" s="43"/>
+      <c r="S3" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="T3" s="32"/>
-      <c r="U3" s="33" t="s">
+      <c r="T3" s="36"/>
+      <c r="U3" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="V3" s="34"/>
-      <c r="W3" s="32" t="s">
+      <c r="V3" s="43"/>
+      <c r="W3" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="X3" s="32"/>
-      <c r="Y3" s="33" t="s">
+      <c r="X3" s="36"/>
+      <c r="Y3" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="Z3" s="34"/>
-      <c r="AA3" s="32" t="s">
+      <c r="Z3" s="43"/>
+      <c r="AA3" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="AB3" s="32"/>
-      <c r="AC3" s="33" t="s">
+      <c r="AB3" s="36"/>
+      <c r="AC3" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="AD3" s="34"/>
-      <c r="AE3" s="32" t="s">
+      <c r="AD3" s="43"/>
+      <c r="AE3" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="AF3" s="32"/>
-      <c r="AG3" s="33" t="s">
+      <c r="AF3" s="36"/>
+      <c r="AG3" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="AH3" s="34"/>
-      <c r="AI3" s="32" t="s">
+      <c r="AH3" s="43"/>
+      <c r="AI3" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="AJ3" s="32"/>
-      <c r="AK3" s="33" t="s">
+      <c r="AJ3" s="36"/>
+      <c r="AK3" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="AL3" s="34"/>
-      <c r="AM3" s="32" t="s">
+      <c r="AL3" s="43"/>
+      <c r="AM3" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="AN3" s="32"/>
-      <c r="AO3" s="33" t="s">
+      <c r="AN3" s="36"/>
+      <c r="AO3" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="AP3" s="34"/>
-      <c r="AQ3" s="32" t="s">
+      <c r="AP3" s="43"/>
+      <c r="AQ3" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="AR3" s="32"/>
-      <c r="AS3" s="33" t="s">
+      <c r="AR3" s="36"/>
+      <c r="AS3" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="AT3" s="34"/>
-      <c r="AU3" s="33"/>
-      <c r="AV3" s="34"/>
-      <c r="AW3" s="33"/>
-      <c r="AX3" s="34"/>
+      <c r="AT3" s="43"/>
+      <c r="AU3" s="42"/>
+      <c r="AV3" s="43"/>
+      <c r="AW3" s="42"/>
+      <c r="AX3" s="43"/>
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
@@ -10406,28 +10136,6 @@
     <row r="42" spans="2:50" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="S2:V2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AI2:AL2"/>
-    <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="AQ2:AT2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="Y3:Z3"/>
-    <mergeCell ref="AQ3:AR3"/>
-    <mergeCell ref="AS3:AT3"/>
     <mergeCell ref="AU3:AV3"/>
     <mergeCell ref="AW3:AX3"/>
     <mergeCell ref="AA2:AD2"/>
@@ -10441,6 +10149,28 @@
     <mergeCell ref="AA3:AB3"/>
     <mergeCell ref="AU2:AV2"/>
     <mergeCell ref="AW2:AX2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="AM2:AP2"/>
+    <mergeCell ref="AQ2:AT2"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="Y3:Z3"/>
+    <mergeCell ref="AQ3:AR3"/>
+    <mergeCell ref="AS3:AT3"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AE2:AF2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>